<commit_message>
ADD Stage-1 Stage-2 A1-A20 tasks
</commit_message>
<xml_diff>
--- a/VladDevv/evidence.xlsx
+++ b/VladDevv/evidence.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\6. Vlad DEV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\0_6. Vlad DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,45 +57,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -142,6 +109,207 @@
   </si>
   <si>
     <t>omniflix1kw75spqdu6xcc2qjzm2c8qqrv66asv7q9eed0r</t>
+  </si>
+  <si>
+    <t>C1C38CDA8288E9B16CAF4AABA8263DB8838A454BCDA860DF47ACECDDFFA5D52B</t>
+  </si>
+  <si>
+    <t>devNFTGO</t>
+  </si>
+  <si>
+    <t>3AD8D69DB0427EAD7DCCDCB11625095F9635C4343DECE2E0F09871247DAC42C0</t>
+  </si>
+  <si>
+    <t>dev001</t>
+  </si>
+  <si>
+    <t>6E4A274F517B563B666BD4062F89C1A75A4498DA8BE6FBDD3587757E3D437178</t>
+  </si>
+  <si>
+    <t>dev002</t>
+  </si>
+  <si>
+    <t>DAF3864103B6B56AC129F5F66512B5E6C9083D7ACD413621DE62630114DAAC2D</t>
+  </si>
+  <si>
+    <t>dev003</t>
+  </si>
+  <si>
+    <t>DD9C518531C18771E1C7E193BC51D379ACF7152B716678804FCBD1912136D731</t>
+  </si>
+  <si>
+    <t>wasm.juno19us6395gfz2ehej6yj4hzv52zzpmwt55xy6e6xapd2a8lp3twltqpprnz7</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>D034EC4C2BD9BA641083D4B9FC40D821580924875DD34294D146134B7E60A4AF</t>
+  </si>
+  <si>
+    <t>ibc/6D80137C833385CFE7DE3167E648DF744D82371868F0BFB3336252DA4FC53D55</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>771F822CBAD7866A21622829F7B3E3CB172D5799D60CFFB7C76275BDD81D8EEE</t>
+  </si>
+  <si>
+    <t>9377C3D8ACB2F3272110186F703D7BD33BE72342D0B4435BBE344D880C4DEF19</t>
+  </si>
+  <si>
+    <t>ibc/F92B236D6E3DA6FD2D9F83065F9B2CD8CF954456B57855BBD2A3812EEFCFC5CE</t>
+  </si>
+  <si>
+    <t>dev007</t>
+  </si>
+  <si>
+    <t>ibc/D51F3EA36A9882F396E1C9C36CEBD5CA901C50A0F192414486BDBAE5F6FB7CDA</t>
+  </si>
+  <si>
+    <t>dev008</t>
+  </si>
+  <si>
+    <t>ibc/155FD45DC0D8DFD3C4508D4F25BFB0550F88D54ECEB727334C809C941928A6C7</t>
+  </si>
+  <si>
+    <t>dev009</t>
+  </si>
+  <si>
+    <t>ibc/1D579AE03B76F6700BACCA7E2A943FA4A686B4773A62238DEBBC8E401EB25361</t>
+  </si>
+  <si>
+    <t>dev0010</t>
+  </si>
+  <si>
+    <t>ibc/2F18680017C266612A4F3B51ECADB784C67ECB7C67CE0E009BFAB273733318AC</t>
+  </si>
+  <si>
+    <t>dev0011</t>
+  </si>
+  <si>
+    <t>ibc/D79A02E6E4522D931A1492327652FB9948A7E88A23ABF7C6D30808D883151754</t>
+  </si>
+  <si>
+    <t>dev0012</t>
+  </si>
+  <si>
+    <t>B1677D247C289A4D86BCFFDAE4E5F24554D23E893A4A5DF7DE951E7DCD0E068C</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>C7DDFA7B5F867461B520A16B1A9232E1D825CE2CAF20CCE7BF2C1714BCCD61EB</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>6D874A9BF2DDC442C1ED23F4F0B912DB05CA84F1F4AFBBA73DAE02AA0B69B4BA</t>
+  </si>
+  <si>
+    <t>4652C5F6DF2F05F34E97AF12952F11C9AB7588E34E59D39AB5E809F024BA0CA9</t>
+  </si>
+  <si>
+    <t>DCEA789F26859EC2DA9760CB0571018B71D833468DB80E45CC2C895297DF1F8E</t>
+  </si>
+  <si>
+    <t>D21BE8AF29800D59B81E0DC152900541D4584E3A9F69E650206FFECF58CF0CE1</t>
+  </si>
+  <si>
+    <t>32A88445D71D7C4E72F7222633CA244883B3A2EB685C8A28AAB24D7466D5386E</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>4CD8D62C2067571CF933493F701B022C4B8A754D9F1AB172752CF61D6B481307</t>
+  </si>
+  <si>
+    <t>23A953552B627AF1BE16B50295C465E07CA40E63EDCDB97CE69C272C651829A5</t>
+  </si>
+  <si>
+    <t>FB30E6458B518C13CE08A4B83EB4E42C17232F7D2967E98E1CDB4173B601EED9</t>
+  </si>
+  <si>
+    <t>AB4400FEF16072BF88EF34CF947E1608030A81986530626363D6CEBD5A02495C</t>
+  </si>
+  <si>
+    <t>0505F9678D19074BEBA9836E0416F2891ED97817312E3641AEA8FE79AA0D8AF5</t>
+  </si>
+  <si>
+    <t>878DB9C76056E99C2A7C223EFC7E1B2A21A72B31EE85B598AA26169CE0CD441D</t>
+  </si>
+  <si>
+    <t>5AB5FAFECE9EA653468B3E1FD7B894BF8AF6E0FC5DFD69DA2E7B8F410F5E676E</t>
+  </si>
+  <si>
+    <t>97D656175AD9D2053CBE1DC5250C28C3D31299972EC3CE7BF150CF5E80E745D7</t>
+  </si>
+  <si>
+    <t>5FA957003C84CB8DA0518D0D612BDBE7726881987C89B3616381472CE3E75C71</t>
+  </si>
+  <si>
+    <t>878FD2071A1E0C4230A65E16FAA56FE20801253F9FC0A88B3C000AD0401236DB</t>
+  </si>
+  <si>
+    <t>E4A21A4D49185D5BD793FA9E6F1AF3B666C34ED196AA799CD12ED0C2F412DF35</t>
+  </si>
+  <si>
+    <t>A1030D528015D636C85B7DF5332386D05C5650E926C2B4C0A9D1A7D7359AB64E</t>
+  </si>
+  <si>
+    <t>3CD69B6A546377D239B0D81EE95391301203020E78A0706A77BCFB502B510868</t>
+  </si>
+  <si>
+    <t>AEE08F81F2F8A30A9FCE99831333361720E03910AF2FE91CB8EB61D28C5053F7</t>
+  </si>
+  <si>
+    <t>3F8EB4BF122EE7CC28796BD7ECAAB561334A08929A0A39A4FE218A5F15CA6A34</t>
+  </si>
+  <si>
+    <t>3D1A2A774596A692011B83D6A0CB95A7BDB85A86F332072BEC3C3D2768AC5CE8</t>
+  </si>
+  <si>
+    <t>91E0E0D757F641444BE2F6F390D7C1364E12D2D82EF1AB03D80038A742F61035</t>
+  </si>
+  <si>
+    <t>036F9BD06C774994FFDD905FF1C00F6C50B6A1EF5A44F85DEA38382CF08D811C</t>
+  </si>
+  <si>
+    <t>C6CE80E306B323AB78C8A890D810DE91C351C33A3056606B1FC4EB28DEEC3CAA</t>
+  </si>
+  <si>
+    <t>539193C37810492D8DAAED414D27D2F5E5E7ADE96AA5EE905AA9394FC1AD2651</t>
+  </si>
+  <si>
+    <t>46CDB53B1D71CB67A3166B3DE25CFA7AA2EFFE8AF667E59C695B0B0D1A521B25</t>
+  </si>
+  <si>
+    <t>BCE0C1B739081C90C6022125F466F23E88E7A3F65646A5E0A12EDE258F88DD0A</t>
+  </si>
+  <si>
+    <t>6D305ED7E4B796F90783D701950AC18769A0AAFC032DC048863B0FFB3E0DC458</t>
+  </si>
+  <si>
+    <t>AFC82574B33C0454A186BDC1A14D6FE322069C0AC649C844527CCCD82A154A8C</t>
+  </si>
+  <si>
+    <t>A014F6E1A13382D1152BC0759018D88F53F71A20401B4DD5EC54F0EB06A70C37</t>
+  </si>
+  <si>
+    <t>9EC0F75A09FC44F595184B313B1A4593D644E1D757CADDF95EC9CCC1AFD12F04</t>
+  </si>
+  <si>
+    <t>B695CE9338D6AE22D724FC0244284242F429966623416E9CCE965A0C89F3109E</t>
+  </si>
+  <si>
+    <t>0E357F164C6FB4B4D958A87D61DDD7FA4E34916DCB79D307B310049C87DCD8E2</t>
+  </si>
+  <si>
+    <t>1F97CC5A1279FB4D94FB0B612EB66034499E7E038788C7B8EDC465AE680E119D</t>
   </si>
 </sst>
 </file>
@@ -538,7 +706,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -556,54 +724,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +787,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -629,18 +799,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +825,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,18 +837,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +863,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -701,18 +875,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +901,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -737,18 +913,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -761,9 +937,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,23 +959,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -809,9 +999,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -829,23 +1021,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -857,9 +1061,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -877,23 +1083,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -905,9 +1123,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -925,23 +1145,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,9 +1185,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -973,23 +1207,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1001,9 +1247,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1021,23 +1269,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1051,7 +1311,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,19 +1325,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1084,9 +1347,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1104,23 +1369,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1132,9 +1425,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1152,23 +1447,55 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,9 +1643,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1331,22 +1660,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1360,7 +1716,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1374,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1385,16 +1743,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1767,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1423,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1434,16 +1794,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1458,7 +1818,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1472,10 +1834,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1483,16 +1845,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1869,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1522,10 +1886,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1533,16 +1897,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +1921,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1567,22 +1933,23 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1593,7 +1960,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1603,18 +1972,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>